<commit_message>
Get daily reddit data: Tue Feb 18 08:10:49 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_23.xlsx
+++ b/data/collected_data/2025_02_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C494"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3287 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1is5koa</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Weak Nails</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1is5koa/weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1is6u7q</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Really proud of the length and shape!</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ul4zlayajuje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1is6tkn</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>don't get mad</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is6tkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1is6rha</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Duck Nails</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is6rha</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1is6nse</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>My husband told me to get my nails done, and this is the result. Love it 🌸</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is6nse</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1is6b4g</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>I loved this set, i hope understand it 🫶                           🧊🚛            &amp;              🌊🛥️</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp1hxlc3duje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1is56pl</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>I did these on myself!!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sn0f79vk0uje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1is3stn</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Expectation vs reality: honest opinion?? 😭</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is3stn</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1is508x</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>First XS Almond Set 💗</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amu4necoytje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1is4o7g</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Simple but pretty 🌸</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddmbygp7vtje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1is4dbf</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>What’s the best kind of gel/long-lasting nail polish option for weak and brittle nails?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1is4dbf/whats_the_best_kind_of_gellonglasting_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1is3ubi</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>The sets I’ve done recently!!</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is3ubi</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1is3qws</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>obsessed with my blue aura nails! 🌀</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hstein28mtje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1is3o7d</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>LPS press on WIP</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz9ddnrhltje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1is35jg</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>I think I found the perfect design. Rose with daisies</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxgxgl2lgtje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1is34x8</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Nail length differences</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is34x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1is1rq8</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Builder Gel with cat eye</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nippgldz3tje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1is0yw4</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Nails I did this week</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is0yw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1is1e7l</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Wicked x imPRESS Destined To Fly (press-ons)</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is1e7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1is1apb</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Did some strawberry nails on a friend 🥰🍓</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is1apb</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1is18rz</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Will a thick coat of gel help with breaking?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yniwohazsje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1is0mq1</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>These are the press ons I did today the first one bunnies cause my username is Sher.bunny and blue&amp; pink are my favorite colors and the third picture is my inspo for the second, from yana on Pinterest. But with a couple different things like the cherries. First time I painted eyes! How do they look?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is0mq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1irx4ua</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Need some pointers about press-ons</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irx4ua/need_some_pointers_about_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1irzaui</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Going back to natural nails question?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irzaui</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1iryhyb</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>What do you do with the leftover tips that don’t fit you?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iryhyb/what_do_you_do_with_the_leftover_tips_that_dont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1irvova</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Nail is broken - Is this something I can save with acrylic?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxg6upj0rrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1irww0j</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Nail glue alternatives?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irww0j/nail_glue_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1irx30p</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Allergic reaction</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irx30p/allergic_reaction/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1is0op8</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>My engagement nails 😊✨💜</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6ay9hqhusje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1is0lwd</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Velvet: Mooncat Death Star</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vi2k55kutsje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1is05y4</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Finally found the perfect dark red color I’ve been dreaming about for years</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jb0b714qsje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1is03yb</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>bright blue💙</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is03yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1irzc3x</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Rate my set! Silver ombré set</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irzc3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1irz7xh</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>This week we got my Matte-Chrome, Bejeweled 5XL Gel -X Nails</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irz7xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1irysty</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>2nd set of press ons?!</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irysty</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1iryfn1</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>solution to stop biting my nails</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejd9thwjbsje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1iryaoi</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyg4c7pjasje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1iry3fk</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Sweet as berry pie</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r4sz37x8sje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1irxczb</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>hello everybody! i hope this is the right place to post. looking for help with my natural nails!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irxczb</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1irx3nj</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>I live for galactic vibes</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iiw2nxod1sje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1irx302</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Super cute cheetah print on natural</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqvuat391sje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1irwyzm</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Flowers</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68ok450f0sje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ird7i6</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Query</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dmre0wj4nje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1irwt7u</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Lookin at my fresh mani while waiting for an ultrasound is nerve calming 💜</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s7uifm7zrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1irvjgy</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>My sister just had these nails done, aren't they very beautiful?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/av4l9guwprje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1irwl0t</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Best gel glue for press on nails</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irwl0t/best_gel_glue_for_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1irwjyt</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Some press ons I’ve made! Still learning</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irwjyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1irwhv1</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>My Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4elkiywwrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1irwgdw</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Kinda fall vibes but I love them 🤎</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irwgdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1irweha</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Bejeweled Nails✨</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irweha</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1irw4s7</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Need advice for a starting point in un-ruining my nails.</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8l8b54x8urje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1irvvkd</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Just finished my 2nd set ever on myself and I really like it</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irvvkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1irvuka</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>making my own press ons!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r4u3na6srje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1irvtdr</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>press ons for my sister:)</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3mvhxkxrrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1irvmed</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Cat eye Polish with butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irvmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1irve4a</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Best way to fix lifting sides?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irve4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1irv4qq</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>my friends new nails! 🤎🤍</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcjnx7qzmrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1iruuu0</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Valentines nails ❤️</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0nbu7qs1lrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1iruome</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Really i love It!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtv6bruujrje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1irulkb</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Perfect Nude</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsymq819jrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1irtt3d</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>First time trying press ons! What do we think?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch4l9igidrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1irtgby</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>I hate all the tips that go to waste</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irtgby/i_hate_all_the_tips_that_go_to_waste/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1irt0hw</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>I do nails for free recently did my friend's hands. What do you think?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irt0hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1irsy58</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Any advice for shaping weird nail?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irsy58</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1irsrl0</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Thrilled with these!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irsrl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1irsl9h</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>is this as bad as I feel like it is</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtcnxt0y4rje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1irsi63</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Zero 🐕 👻</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irsi63</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1irryaf</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Capybara can you tell? Or does it look like a dog? I did what I could</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnz1ov9f0rje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1irrvy4</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>At home natural nails</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irrvy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1irrqjs</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>I did my own nails!!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d5pc99fyyqje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1irrpxk</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Milky white nails 🤍🥛</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irrpxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1irqs5t</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Tools for putting nails on?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irqs5t/tools_for_putting_nails_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1iroj9v</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>UV lamp</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iroj9v/uv_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1irj9m9</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Brazilian nails for Carnaval</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uop01x986pje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1irqpd0</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>One of my all time favorites: Voodoo by DND</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cm7vkrmrrqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1irpy2z</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Cat-eye mani at the airport</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irpy2z/cateye_mani_at_the_airport/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1irq0kq</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Help! Is this my cuticle or just dry skin along the cuticle line?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irq0kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1irpk1s</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>The idea VS the product</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irpk1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1irp73v</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>I love my new set.</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjjfqrrahqje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1iroqch</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Barbie Outfit set</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iroqch</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1irojzw</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Nail lamp</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trig1aftcqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1irobxc</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Fresh set!! 💐</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8x7j7k36bqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1iro8u5</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>bath procedures and fresh manicure. My favorite feeling</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pe9q68b9qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1iro2km</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>my favorite design ive had (so far) (it is my design)</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iro2km</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1iro2iw</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Just tried doing something myself</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5g3vn5r89qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1irnwop</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>OPI 'Defying Gravity'</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn6jlpe28qje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1irnlt7</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>i call my nails talons</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irnlt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1ire6o2</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>What happened?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ire6o2</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1irfjk4</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Press on’s insane durability</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irfjk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1irg6n8</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Can you use “gel tips” without doing the whole gel process?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irg6n8/can_you_use_gel_tips_without_doing_the_whole_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1iri9t3</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>We can stop crying now! 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iri9t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1irngw3</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>What type of nails should I get?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irngw3/what_type_of_nails_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1irlwwt</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Cute little set I did yesterday (hard to photograph)</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erm7mn50tpje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1irl5c2</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>white clouds at nail tip?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irl5c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1irk4k4</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>DND Indigo Wishes😍</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtd41ci3epje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1irjuj3</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>What is an “acrylic pink and white” set vs “acrylic?”</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1irjuj3/what_is_an_acrylic_pink_and_white_set_vs_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1irnhll</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Snake</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kymexx605qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1irn8jq</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Blue nails</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sg2agr43qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1irmvec</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>First time doing at home gel tips</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ap6qglue0qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1irm3io</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Valentines nail set</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0dp6v2zfupje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1is6mws</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1is6mws/what_should_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1is4qbx</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>ILNP Roulette (velvet)</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2w8txg9tvtje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1is4fop</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>A little coquette action for Valentine's Day (late post I know!)</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is4fop</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1is42nq</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Day NINE wearing this and it's still perfect. I'm dreading taking it off though</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is42nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1is2k8f</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>got my nails done first time</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1is2k8f/got_my_nails_done_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1is1x3r</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Mooncat This is a Storm Warning</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is1x3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1is1gf2</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Slowly turning into claws (hook/ beaky) - is it the nail or the technique? Scroll for pics</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is1gf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1is1cab</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Nails in 2020 vs today</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is1cab</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1is1aou</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Alibi</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xqqj62szsje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1is186p</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>I can’t get over this polish</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is186p</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1is0iex</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>this is your sign to go buy zoya’s venus 🤩🤩💫</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s8vkmb4zssje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1is01zx</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Jumpsuit orange in DC today</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is01zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1irzobn</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>I bought a bottle of ORLY Beautifully Bizarre at Ulta and was VERY confused when I saw the polish on the website.</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irzobn</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1irz9lt</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Polish Allergy?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1irz9lt/polish_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1irz8k0</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Curse of Calypso, you are a beauty ✨</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irz8k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1irz5b6</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsecf4ujhsje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1iryw59</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>🍎 forbidden fruit 🍏</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iryvp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1irydyr</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Essie - Leather Weather</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irydyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1irydxh</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Winter Citrus Skittle &amp; First Attempt at Nail Art</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irydxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1irxrfb</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Where to buy Essie smooth-e ridge filler base coat?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1irxrfb/where_to_buy_essie_smoothe_ridge_filler_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1irxh3q</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>How to destash in Europe (excluding UK)?</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1irxh3q/how_to_destash_in_europe_excluding_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1irx8az</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>She’s a bit of an attention whore 🤹🏼</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fv8hkthd2sje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1irx6ky</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>New to stamping. I don't know how to properly clean up around the edges especially when using black. It just seems like I'm smudging it all around. I have an angled brush and been using a q tip but I don't know if im doing it right? Are there other tips? Should I put my top coat on before I clean up</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irx6ky</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1irwu3h</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>It Can't Rain All The Time</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irwu3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1irwg3q</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Belated heart mani</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irwg3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1irw5iv</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Prism Polish never disappoints</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irw5iv</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1irvs4x</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>how do we feel about the green?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irvs4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1irvdma</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Sky Fire</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4ia95tporje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1irv9g4</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Let’s see those nails and fur babies!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irv9g4</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1iruov9</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Anybody else's nails break MORE when almond-shaped?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejwqqrgujrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1irtlci</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Valentine’s 2025 Mani #5: Ahmya Cosmetics &amp; BKL</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqx5ljnzbrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1irsznf</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Something different after all the Valentine’s Day pink</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c2wm9m2s7rje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1irsjp6</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Zero 🐕 👻</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irsjp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1irrv2n</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Makeshift with Magsafe</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zvct16vszqje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1irroid</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>If you love a flakie jelly, clap your hands 👏</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irroid</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1irrfq3</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>My “how is it still winter” manicure</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrlv5l4wwqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1irr2lp</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>DVN From the Wound + Orly Bohemian Child</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irr2lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1irqt5b</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Very Virgo shorties</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eue50ephsqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1irqrg1</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Green for spring but still a bit frosty</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/884c2qy5sqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1irqaqg</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Nail dust collector under €100</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1irqaqg/nail_dust_collector_under_100/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1irpst0</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>My Wife Picks My Mani: Part 8</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irpst0</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1irp38r</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>My first Kathleen and Co polish 🤩</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4jcqz1fjgqje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1iropmb</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>My “it’s not spring yet” nails</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om51r1gwdqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1irobmv</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>My first EdM order just shipped and I had no idea we live in the same city, gonna be the fastest shipping I’ve ever had 😅 what’re your fav EdM polishes?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kedqqfw3bqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1iroa55</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Experimenting on myself: PVB in the polish with non-PVB basecoat</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iroa55/experimenting_on_myself_pvb_in_the_polish_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1irnx6k</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Rainbow trout :)</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irnx6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1irngk4</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb3vij1s4qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1irnbz4</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Can we just pretend that it’s spring? 🌷</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmblxbus3qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1irmwkh</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Dash of galaxy</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irmwkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1irm9co</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Cant get over this color!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbhfdqcpvpje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1irlnyj</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Added some sparkle to my shorties with Zoya - Tamiah</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irlnyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1irljg6</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Best Base/Color/Top Coat brand combos - long lasting?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1irljg6/best_basecolortop_coat_brand_combos_long_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1irl30v</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Please suggest your favorites from LynBDesigns!</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1irl30v/please_suggest_your_favorites_from_lynbdesigns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1irkoqo</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>accepting the cold hard truth of green polish?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irkoqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1irkjzf</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Recreating blue sand nails with regular polish</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ledhqmjuhpje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1irkjd2</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Zoya FeiFei on brown skin</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3miwzcsohpje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1irkhuj</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>💛🗡Kill Bill🩸💛</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irkhuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1irjk8k</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Is this shape working for me?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irjk8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1irizay</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Had to get up early and do some stuff with a personal trainer that I was super nervous for today 😅😅 at least my nails are a pretty color 🌀🩵</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdyd70ba3pje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1irixf2</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Nude base under sheer polish reccs?</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irixf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1iriitd</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>✨Woman in STEM✨</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzdrfj1dyoje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1irhkqq</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Unreleased Prototype</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2z886jjnoje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1irhe0e</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1irhe0e/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1iqx9ey</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Holo taco peely base</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iqx9ey/holo_taco_peely_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1ir1q8a</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Neon Pink</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ir1q8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1is4pk1</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>practice makes perfect</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zp110p7mvtje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1is33rj</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I can't tell if this is good or if I just wasted my time</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhoanzj4gtje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1is1rqm</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Sparkles n' swirls ✨🌀</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6toh2kz3tje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1is0eqt</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Black &amp; Red</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idbt6hr4ssje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1irzvni</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>diy evil eye nails 🧿</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nagq57wpnsje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1iry9y5</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Turns out, I actually don't know colors</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iry9y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1irw3ga</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Que opinas de estos?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wd4rlg0urje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1irv7g7</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>They like it or they are very simple</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/juqme1jinrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1irtty1</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Vacation Press Ons 🧜🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw1y4vkodrje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1irsq0m</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Some of my press ons!</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irsq0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1irspwu</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>one of my favorite designs of mine. i love my talons. this is my design. my hands. i hope you like it :’)  inspired by the trans flag + lgbtq flag &amp; frog patterns.</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irspwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1irsavt</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>DND polish list?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1irsavt/dnd_polish_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1irq8yl</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Tried chrome and I have questions</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vwr0aknoqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1irplgy</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Foil flecks</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gv7i1875kqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1irpc7y</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>When a ladybug lands on your picnic blanket type nail</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irpc7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1irorn8</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Barbie Outfit set</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irorn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1irnoz5</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Concept is good the execution is….. something</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irnoz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1irn4wp</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Feb 2024 vs Feb 2025 🥰</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ju4k2zif2qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1irmyg3</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>What is everyone's favorite gel they use for cleaning and priming their brushes?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1irmyg3/what_is_everyones_favorite_gel_they_use_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1irmyd0</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>What is everyone's favorite gel they use for cleaning and priming their brushes?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1irmyd0/what_is_everyones_favorite_gel_they_use_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1irlbad</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>My nails for Valentines</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9txccob9opje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1irlfoh</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irlfoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1irl4p1</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Too lazy to finish it haha</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tzlk5cqmpje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1irk1fk</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>More little hand-painted mushrooms 🥰🍄</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fmxfs2cdpje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1irjwxt</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Just trip nails💅🏻</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y5f3jl6cpje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1irjkqn</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Valentine's ❣️</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2ppaca39pje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1irjew5</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>wet slimy moist alien themed nails 👽</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wp3iaauj7pje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1irg5hi</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Frosty Nails❄️</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irg5hi</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Feb 19 08:11:02 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_23.xlsx
+++ b/data/collected_data/2025_02_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C494"/>
+  <dimension ref="A1:C684"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8831,6 +8831,3236 @@
         </is>
       </c>
     </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1it0c5o</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Sunset beach</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it0c5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1iszr42</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Tried red today:))</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iszr42</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1iszbwv</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>what is this vertical crack looking line on my fingernail?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzrn0x34m1ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1isz47k</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>These nails are too girly and I love it</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b72ml1wlj1ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1isz4cn</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Claws I did for the Aespa concert in Chicago</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isz4cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1isz138</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>new nails (made by myself)🤍😍</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isz138</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1isy4u3</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Should this be happening after a week?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isy4u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1isxc9s</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isxc9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1isx8wh</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Nail polish never smooth</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1isx8wh/nail_polish_never_smooth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1iswupq</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Help!!!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yeohh44qv0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1iswj1k</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>I’m obsessed with these nails! 😍</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5oswp2ais0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1iswp8m</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>i’m wearing holo taco one-coat black &amp; i am obsessed!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ak7a2sfau0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1iswp21</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Practicing nail art today. Not a cohesive set just individual nail art. Seeing what I could paint on a small canvas :)</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iswp21</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1iswobr</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Last valentine nails of the year♥️✨</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/793b9ln1u0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1iswg71</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Hard gel</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iswg71/hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1isw2wy</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Obsessed with meeee</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isw2wy</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1isvvz4</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Harry potter order of the phoenix nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isvvz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1isvf3v</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Vampy Red Cat Eye with “Hidden” Thumb Art 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rnggixaki0ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1isvb2b</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>prettiest nails ive ever had by far 😍💚</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/abcpcjkkh0ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1isv7j5</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Day 3 and gel nails chipped</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gnzdgcrg0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1isuzi8</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Valentines '25</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isuzi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1isukz8</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>first time painting something with a face :)</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cwyj6f9b0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1isug8a</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>My fav Jan nail set. Do you prefer nude or bling rhinestones?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isug8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1isud7f</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Feb nails</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kl755m1c90ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1istsf3</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Have been trying to figure out how to emulate the packaging of my favorite lip gloss and finally did, should I keep it matte or go high gloss?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n16zd0mn40ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1isteh8</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>what is this?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wem0x7hg10ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1ist7dn</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>In love with this current set</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd1qpa0tzzje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1ist1mn</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Pearl nails for vacations 🐚⛱️</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf8oqshiyzje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1iss9jz</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Question for the nail techs</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iss9jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1iss79s</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Moody blooms inspired nails</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5zpf53rrzje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1iss5tm</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>astrological charm gel x set for me by me on me</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08qwzpxerzje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1iss1yd</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Can’t post February nails without January! Dreamy nails to kick off 2025 💅🏼✨</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vs9miehiqzje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1isruw8</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Post Valentine’s Day nails — trying a ballerina shape over the usual almond 🩰</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtbdvtsyozje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1isrtmi</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Ist daily charm vegan?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1isrtmi/ist_daily_charm_vegan/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1isrjgu</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Did a cute lil Valentine's Day mani</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmbjng3imzje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1isr4ik</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>What nail products can I use?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1isr4ik/what_nail_products_can_i_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1isrhty</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>First attempt at valentines nail art</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isrhty</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1isr3ca</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Does this color work for me? / Essie 'Caught in the Rain'</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isr3ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1isqtx1</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Tutti fruiti🍒🍓🍋🍉</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isqtx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1isqro0</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Arcane Nails!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1isqro0/arcane_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1isqbko</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>So fresh &amp; so clean, clean 🤍</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k5qqfyzczje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1isq9yh</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Cat eye stiletto</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fbsgko2sczje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1isq16h</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Russian manicure or sculpted nails in Oakland?!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1isq16h/russian_manicure_or_sculpted_nails_in_oakland/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1ispzwo</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Nail Advice</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m56gr63qazje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1ispwms</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Celestial Designs</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ispwms/celestial_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1isppzj</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Black with foil</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru8vyg2s8zje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1isp7md</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Painting a Billie eilish set for myself 💙 Here she is</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zfqvehg5zje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1isp36t</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>I am never going to financially recover from this 🐯</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isp36t</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1isozx4</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>UPDATE: Worse than I thought 😪</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isozx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1isoxcx</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>new set</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isoxcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1isowmw</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Cherry chrome</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isowmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1isossb</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>🖤 🩷</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isossb</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1isok66</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Getting better</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/accxaem2wyje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1isok3f</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>The YumEarth special 🍬🍭</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isok3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1isoho7</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Finished product… honest opinions?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvgty0okvyje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1isoe95</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>abstract green and orange nails!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isoe95</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1isnvxg</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Did a French tip for the first time. It was…..not easy 🥲</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isnvxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1isnp8u</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Very girly nails 🎀</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ekehc42qyje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1isndtr</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>nude with some twinkles ✨</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y29udt0unyje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1isnd3r</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Star destroyer</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isnd3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1isncub</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Very simple</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xuw5h6omnyje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1isn7cq</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Nails for the month of Feb 🍒💕</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isn7cq</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1isn796</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>3d, chrome and tattoos.... Winning combo!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cv9301pgmyje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1ismwam</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Does reshaping gel x tips actually cause retention issues?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ismwam/does_reshaping_gel_x_tips_actually_cause/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1ismg22</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>First time getting my nails done as a man</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj1ay9r2hyje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1ism3fj</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>In love with my newest set!</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pipivbzleyje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1islf6y</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Advice for Nail Doing!</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1islf6y/advice_for_nail_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1islxsx</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>How can I improve the cat eye I’m going for? I only got a small round magnet..</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujgt06shdyje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1isls6k</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Beetles Gel Merlot Wine- deceitful</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isls6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1islpxh</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Plaid nail stamping</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1islpxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1islfmg</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>GEL BRAND ADVICE PLEASE😭</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1islfmg/gel_brand_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1isl00w</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Ideas with transparent base?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zg389nr6yje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1iskwk7</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>New nails. Love these colors.</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45aaopz26yje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1iskvp3</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Dupes for Game Over??</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iskvp3/dupes_for_game_over/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1isizbj</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>How many weeks?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isizbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ishgw6</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Do you think square nail would fit me ?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ishgw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ish7rs</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Coffee Inspired</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ish7rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1isfrk2</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Brittle Winter Sadness inspired fluid art 😅</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isfrk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1isk145</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>🔥 My feelings will not be repressed. You must allow me to to tell you how ardently I admire and love you.</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ghvb70c00yje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1isk9pz</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Picnic themed nails 🐜🍉</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isk9pz</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1isk6hp</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Neutral pastel rainbow 🩵🩷</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isk6hp</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1isjruu</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Todays project 🥳</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m3ov2s9yxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1isjld8</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Primera vez que yo misma hago mis uñas.</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzrmz671xxje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1isjffg</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts Box Art Kairi as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isjffg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1isja8r</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Code red, help😭</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1isja8r/code_red_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1isj1t2</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>First “basic” set I’ve done since July 🩷</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isj1t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1isilej</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Which shape suits me better?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isilej</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1isi7y1</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>It is still Wear Red for Heart Disease Awareness month</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69sofcscnxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1ishy9n</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Late  Valentine’s Day Nails ♥️</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7x4zms1hlxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1ishdn0</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Does this dip mani look bad/bulky?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ishdn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1isdniy</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Nails need repair</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isdniy</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1is7pnd</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Damaged Natural Nails</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is7pnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1isbqfd</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Onychocoliosis</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2horucze7wje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1isfru1</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Suggestions for Russian Mani Classes?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://luxynailsandbeauty.com/products/russian-manicure-for-beginners</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1isajfn</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Gel Polish/Dip Powder: What am I missing?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1isajfn/gel_polishdip_powder_what_am_i_missing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1isgua6</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Man, I love chrome 💕</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/481gumuidxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1isgo9h</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Pls help</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fokuiwsbcxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1isgmx2</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Gel Lamp Safety Help!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isgmx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1isgh4u</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>ASP Ravishing in Raspberry</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyhvdw5waxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1isgdjl</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Why does this happen???</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crhud9v5axje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1it008l</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>After a decade of gel, I’ve come full circle back to my first love! OPI Princesses Rule! was my first “nice” polish that got me into nails 💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isxl3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1iszk02</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Anyone else hate posing your hands? (A Series)</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iszk02</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1isyozx</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Polish Me Silly, Gee Willy!!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isyozx</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1iswt9g</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Mantener uñas limpias</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6d3oiacv0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1iswnlz</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Many air miles but omg</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcd8qpput0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1isvedk</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Fishing lure nails 💅- again!</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isvedk</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1istjis</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>You can’t go wrong with wine.</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1istjis</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1ist5rm</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>mooncat collection</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40lhwigfzzje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1iss7gl</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Mid-Afternoon Glowstick</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iss7gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1iss3k9</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>my first time doing the velvet effect!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iss3k9</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1isryhc</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Holographic + jellies = all the possibilities!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isryhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1isrqg0</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Removal question</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1isrqg0/removal_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1isr5hl</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Guiding Light 🩵🩷</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isr5hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1isr2lh</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Rainbows!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isr2lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1isqxgw</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>that sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6a7b5ibphzje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1isquzq</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat Sabertooth</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1isquzq/dupe_for_mooncat_sabertooth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ispsp0</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Took off builder gel nails and my natural nails are essentially ruined.</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ispsp0/took_off_builder_gel_nails_and_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1iso8yp</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>God I love this colour sooo much</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iso8yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1iso1p9</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Nailtique in Canada</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iso1p9/nailtique_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1isnqoz</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Haul photos, because y’all get me</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isnqoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1isng4k</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>2024 Nails Recap 💅🏽</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isng4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1ismwdk</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Favourite pink from ILNP?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ismwdk/favourite_pink_from_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1islwp0</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Favorite Base Coat / Essie Smooth-e Replacement?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1islwp0/favorite_base_coat_essie_smoothe_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1islgh2</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Polyvinyl butryal recovery club</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1islgh2/polyvinyl_butryal_recovery_club/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1iskrwa</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Does anyone else have trouble with polishes bought at TJ Maxx / Marshall's?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iskrwa/does_anyone_else_have_trouble_with_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1isknjk</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>West Texas Peyote 💜</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uz8bbubc4yje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1iskksm</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>FUN Lacquer - Northern Lights</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iskksm</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1iskfr5</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>OBSESSED - I totally get the hype now</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82r1dexv2yje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1iskcrh</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Deviled eggs, anyone?🍳</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iskcrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1isk1p4</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>🔥 My feelings will not be repressed. You must allow me to to tell you how ardently I admire and love you.</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qq28ap240yje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1isjn0t</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Dearest hubby gave me these amazing cases! So excited</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0nw9ercxxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1isij8s</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Love Hurts</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isij8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1isif6x</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>February is Wear Red for Heart Disease Awareness month.</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k02tnmfsoxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1isi5gb</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Don't normally wear blues but this one I can't resist! 💙</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isi5gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ishevm</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Sheet marks help?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bke4kcqqhxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1ishdel</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Couldn't stop staring at my nails today</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1q7t82ghxje1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1isgeid</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Does anyone have both Lavender Sky and Sheer Tint Lavender?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8gos14daxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1isfqw4</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Brittle Winter Sadness inspired fluid art 😅</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isfqw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1isfc37</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Dupes for Mooncat Moonfairy and/or Moonicorn?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1isfc37/dupes_for_mooncat_moonfairy_andor_moonicorn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1iset8a</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>The one and only 👑</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iset8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1iseama</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Just did the ol' chop chop</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdao488auwje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ise2hb</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>received this as a mystery polish from kbshimmer</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ise2hb</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1isdtxd</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>🍋‍🟩🧊Mint Mojito🌱🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isdtxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1isd4yb</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>i spent 4 hours doing these fruit nails</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isd4yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1iscye1</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Any tips for improving my nails?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mks55a6yiwje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1iscvkp</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Quite possibly the most beautiful nude I’ve ever tried</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iscvkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1isc875</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Top coat to mimic jelly/crelly finish?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isc875</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1isc20b</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>If a jelly is SUPER clear, is it still a jelly?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1isc20b/if_a_jelly_is_super_clear_is_it_still_a_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1isa8zw</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Revlon Moon Candy Dupe/Replacement?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isa8zw</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1is9v6q</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Phoenix Indie - I Wish…</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is9v6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1is9k9m</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Flight of the monarchs 🎃</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6t6qhmiivje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1is9hew</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Glowy greige swatch request - Memento Mori (Mooncat) + Relics of Time (EDM) ?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is9hew</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1irp1hy</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Fandom Flakies Issue</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lh876gp6gqje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1irw8lk</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Looking for an A-England Dragon dupe</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1irw8lk/looking_for_an_aengland_dragon_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1irwai8</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Vintage manicure</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1irwai8</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1is7y9f</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>My LynB Designs 50% Off Order</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is7y9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1irv7t7</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>ISO a shade like this??</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcmup8zg7qje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1iszsk2</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>General advice and tips? Few sets I Liked for examples</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iszsk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1isyycr</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Transfer foil fail</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvg75r1sh1ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1issc56</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>The galaxy in my fingers! ❤️‍🔥💅🏻🪐</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/noc94x0cszje1</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1isw9xs</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Love Nails Inspo</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isw9xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1isuwb1</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>My nails I did yesterday!</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2l3jz9zd0ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1isu4dw</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Anyone else get distracted by their nails while driving?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eqczzjkd70ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1istqb4</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Thank you everyone for encouraging me to finish this set! I hope you like the rest of it!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1istqb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1issc80</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>How to paint on top of 3D nail art?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1issc80</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1isqicm</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Arcane nails!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1isqicm/arcane_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1isqi8d</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>🌿🌸💜 some spring nails</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isqi8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ispxg1</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Cinnamoroll Nails for my friends bday!!</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ispxg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1isp6vq</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Painting a Billie eilish set for myself 💙 Here is billieeee</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/is9b3rxb5zje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1isnafk</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Looking for advice in how to get this effect</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6huu340myje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ismitx</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Welcome back Player 456!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ismitx</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1isme9f</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>cherry blossom reflections</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isme9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1iskimr</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>question for gel x nail art</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iy1lk16g3yje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1isk8rj</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Did these for Valentines</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isk8rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1isk77n</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Realistic jumping spiders</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isk77n</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1isjpz2</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Do you like them? I am fascinated by the delicate</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmkaul1xxxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1isjna2</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Untitled Goose Game Nails</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vto657gexxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1isjhnj</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts Box Art Kairi as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isjhnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1isjczc</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Black and green 🐍</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kq6cwodvxje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1isj42h</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>A ladybug lands on your picnic blanket type nail pt.2</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isj42h</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ishchn</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I think I corrected the bumps on the plad what do yall think (first pic is the corrected ones)</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ishchn</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1isa8tm</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>First attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isa8tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1isgc9w</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Pressons nails not drying</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1isgc9w/pressons_nails_not_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1isf49f</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>I do my nails myself, how are they?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11cfb4so0xje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1isdvrc</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Finally did something other than fish nails!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isdvrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1isdjyt</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Bling be crazy 🤪</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owq5w5l5owje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1isd3fh</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>my recent nails ♥️</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1isd3fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1isb0r2</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>late for Valentines but I still love it</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouhad2mwzvje1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1is9xm3</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Ame este set..Y tu??</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is9xm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1is8gk3</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Finally done! ❤️</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1is8gk3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb 20 08:11:06 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_23.xlsx
+++ b/data/collected_data/2025_02_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C684"/>
+  <dimension ref="A1:C862"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12061,6 +12061,3032 @@
         </is>
       </c>
     </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1ittkjw</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Sanrio nails by me</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ittkjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1itt9tp</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Nail Bed Regrowth - Before and After</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itt9tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1itt2zu</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Worth $75?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t0c2sro8z8ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1itrdxj</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>What type of extensions won’t damage my nails?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itrdxj/what_type_of_extensions_wont_damage_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1itquh6</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Nail studs that don’t do this??</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ii6m51gk98ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1itplba</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>what is this buildup under my nail?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itplba</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1itru75</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>It’s been a while</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qx8t7rwjk8ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1itq5wl</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Y’all am I crazy? The color looks wrong to me.</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itq5wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1itpyud</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Nude ❤️</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itpyud</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1itp3qs</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>How do you get used to nail polish?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itp3qs/how_do_you_get_used_to_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1itpeol</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Finally got my favorite shape!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itpeol</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1itpbgt</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>My nails have never looked so pretty</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itpbgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1itpb5v</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Favorite mani so far! 💕🍒</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itpb5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1itp8p6</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>very nice black one🤭</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/129atbjlt7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1itp7v3</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>How often do you fully remove polygel vs filling?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itp7v3/how_often_do_you_fully_remove_polygel_vs_filling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1itp2k0</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>I don’t know if I hate this design or if I absolutely love it.</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvikuybxr7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1itp2bo</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>First time Almond</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bem816sur7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1itotfg</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Les gusta?!</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t22uhyip7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1itonmj</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Favorite jelly gel polish?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08v11ok1o7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1itoh08</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Cat eye acrylics</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpz48pwbm7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1ito9tt</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>press ons i did 🩷✨</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/24q4peajk7ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1ito17r</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>❄️❄️❄️Black For Winter❄️❄️❄️</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdkr6irdi7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1itnamc</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts Nobody &amp; Sea Salt Ice Cream as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itnamc</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1itn3iw</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Where to cut your natural nails to avoid breakage</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bph3klk4a7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1itmof4</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Love when clients aren’t scared of a matte topcoat</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hniwz35b67ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1itlw37</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>How did you get started as a mobile nail tech?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itlw37/how_did_you_get_started_as_a_mobile_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1itlg41</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>HEMA Free Suggestions</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itlg41/hema_free_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1itkyy8</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Did she do a good job?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxtru6t2s6ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1itlcpb</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Mardi Gras nails i did on my client today!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eqp50j8v6ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1itl9tc</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Daughter did daddy's toenails</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdcjmogku6ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1itl8ud</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Floral cat eye press ons 💕</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzrj9vn8u6ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1itkzqw</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Got a new nail art kit</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itkzqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1itks1r</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Cat eye nails</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0mmxkuiq6ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1itk4eu</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>vacay ready🌺🌴🍹🐠</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itk4eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1itju7u</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Simple blue for the ending of winter and arrival of spring 💐</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itju7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1itjaii</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Getting Better</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f5hogs3qe6ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1itj3qq</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Finally, from 6 week oldies to a fresh set 😩</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itj3qq</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1itixpp</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Square or almond nails ?!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itixpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1itiws3</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Feeling really ecstatic about my new nails, so had to post them :)</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om63xywsb6ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1itifyd</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Second time doing gel nails!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bsyullh986ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1ithd6y</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ithd6y/question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1iti25f</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Clubbed thumb press-ons</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iti25f/clubbed_thumb_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1itia7u</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Looking for the Ideal Set</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6irxma376ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1ithour</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Red &amp; gold nails 💫</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkw362lp26ke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1ithbuc</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Fabric Nails</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ithbuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1itgxlv</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Hii newbie here, can I do a fill in on my nails that were done with “Tip gel super strong” (assuming this is builder gel) using the modelones poly gel?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itgxlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1itgwkm</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>I Couldn't Decide One Color</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itgwkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1itgjhl</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Fresh set after injury</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgv1lrdeu5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1itgfja</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Turquoise sky, what do you think? 🦋</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uqacnolt5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1itgaag</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>First time at the nail salon</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02p2vheis5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1itg951</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Gel Overlays</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itg951/gel_overlays/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1itfyhd</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Light Elegance Jimmy Gel</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itfyhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1itf9t9</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Pink nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/713xrw94l5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1itf4kh</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Recommendations for best press ons for wider nails 💋</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itf4kh/recommendations_for_best_press_ons_for_wider_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1itf14x</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>princess nails with my sister</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itf14x</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1itev93</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Galaxy nails</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ao0clj58i5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1iteqka</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>How do I get a more consistent nail shape?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iteqka</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1iteax2</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Please help</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ia38kzo7e5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1itdtt2</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Subtle Cat Eyes</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itdtt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1itdtbp</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>What is the safest way to get my nails done?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itdtbp/what_is_the_safest_way_to_get_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1iterqs</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>what vibes do these give off</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hilir0ihh5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1iterie</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>While certainly far from perfect, I’m quite pleased with my very first set of gel press on nails</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/js4cazohh5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1iteae5</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>So far this is the nail growth!</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2n6f704e5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1ite6wl</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>For all of the people struggling with nail biting💖</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ite6wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1itdzhs</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>I changed my manicure, do you like flowers?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydozpg0zb5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1itdw9e</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>simple design for my birthday</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itdw9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1itdlxk</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>first attempt to do my own gel</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9zx79ne95ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1itcygm</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>What’s happening here?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8bs521w45ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1itct1p</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Gel x not working</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8755245t35ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1itcfd1</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Press on retention!</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g6v3cn215ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1itci0f</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>My DIY nail arts made with regular polish! What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wtg3wil15ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1itbjxm</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Honduran food 🩵</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itbjxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1itbna6</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>officially despise builder gel</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7u5knednv4ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1itbm74</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>First time trying chrome nails (ft. Cat)</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itbm74</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1itbfqp</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>French will always have my 🤍</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbhlgxt5u4ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1itbdv7</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Thumb nail always cracks when it reaches a certain length, any advice on how to prevent it/why does it happen?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itbdv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1itauat</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Is it safe to use a rubber UV gel  / UV gel base and regular polish? And if so - how?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itauat/is_it_safe_to_use_a_rubber_uv_gel_uv_gel_base_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1itau4s</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Fairyland nails 🌸</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itau4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1itaoug</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>First set of press on nails I’ve ever made. Not perfect but not terrible imo! What do you think.</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytt48902p4ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1itajnb</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Unhappy with my nails</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itajnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1it9z28</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Help 🥲</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1it9z28/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1it9vr7</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Magnetic polish &amp; iridescent powder combo</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hdmsiuej4ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1it8x0y</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>First acrylic set, should I go to the same salon again?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it8x0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1it13qt</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Nails RUINED - how do I save them?!?!?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1it13qt/nails_ruined_how_do_i_save_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1it8oh0</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Fiest time putting anything on my nails opinion ?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hysrmeva4ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1it6mbp</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Valentine's nails (in my country it's Feb 24th not 14th)</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it6mbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1it55w2</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>How to protect nails when removing glue-ons?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it55w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1it2pl9</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My nails finally grew out their acrylic damage, but I can’t manage to have nice cuticles</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it2pl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1it141w</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Jinx nails I did for my best friend! Struggled with the monkey :( And in the second picture is all the nail sets I’ve done in order from left to right. I just started two weeks ago and I think I’ve improved already! What do you think? :)</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it141w</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1it0kxo</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>My first time with almond nails vs the shape I'm used to</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it0kxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1it011e</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>extensions keep falling off</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1it011e/extensions_keep_falling_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1it8e7c</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>🩷🌸🌸🌷spring nails, i think the color is DND ‘blossom pink’</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it8e7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1it8aak</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Aggressive Gel Removal?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7ui3d2z74ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1it7syp</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>I can't stop looking at my hand with these cat eye press-on nails.</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it7syp</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1it74n7</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>I want to start doing my nails but I have no clue where to begin, please help!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1it74n7/i_want_to_start_doing_my_nails_but_i_have_no_clue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1it6jwv</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Nail day is always the best day</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it6jwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1it5j6e</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Nail gel too thick? Cures with holes when I use instructions</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it5j6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1it50ve</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>valentine nails !</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ya9bqzh7h3ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1it4nl7</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Cinnamoroll Nails 🩵</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb4dwg6rd3ke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1it40h6</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Bad mood cured! 🎀 🌊</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6hycspa73ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1itsqu1</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>POV: its 2010 and Katy Perry has just launched her collection with OPI. You spend your hard earned babysitting money on the crackle polish and your mind is blown.</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sshqoic5v8ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1its5nb</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>After purchasing this shade on a whim I think I've unexpectedly found the polish I want to get married in later this year</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1its5nb</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1itr20o</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Back to basics 🤎</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itr20o</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1itpohz</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Mooncat Mani 🐱</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7z0z7t9ux7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1itpo6i</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>First time using a crackled polish:)</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itpo6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1itplxx</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Venomous Indeed!</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ufiwo2n5x7ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1itoa1r</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Wintery vibes from That's a Snow-brrrainer</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itoa1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1itnrw3</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>How to do magnetic polish with 30lb magnet &amp; press ons?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1itnrw3/how_to_do_magnetic_polish_with_30lb_magnet_press/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1itn4ob</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Whoever recommended OPI metallics a few days ago, thank you</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ezrcbwea7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1itmwon</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>April Fool's Fun</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1itmwon/april_fools_fun/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1itmjxv</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Holiday Mani suggestions</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1itmjxv/holiday_mani_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1itlz6n</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Why is Death Valley so expensive?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1itlz6n/why_is_death_valley_so_expensive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1itlvvy</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I peeled my nail WAY too low. Please help. How to even out the nail????</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpipik4pz6ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1itlr9e</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>tj maxx gem!</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75elurlmy6ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1itlfu9</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Hey beautiful people! Does anyone have a pic of the psilo-sibs over black polish?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1itlfu9/hey_beautiful_people_does_anyone_have_a_pic_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1itktdk</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Basecoat Battle game Two</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itktdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1itkp9w</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>blown away, first time trying magnetic polish</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fl1aktzrp6ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1itk5nz</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Are we twinning? Currently wearing Mooncat’s Maelstrom</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itk5nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1itjzrk</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Thermal &amp; UV Color Changing Polish</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itjzrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1itjxrd</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Space-y Flower Child?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itjxrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1iti8i5</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Mooncat’s “Banquet of Breadcrumbs” in various lighting situations on my yellow-toned Asian skin</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iti8i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1itgii2</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Getting better (?) at the velvet effect 🎀</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itgii2</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1itgi5n</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>I Adore Adored!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u07qzo0st5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1itgfq6</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itgfq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1itg527</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Nichibotsu by Phoenix (PPU 2024)</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7psw8hker5ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1itfrey</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>My MIL Picks My Mani?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itfrey</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1itfdhb</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Such A Farse - EdM 💕</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52woeg8vl5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1itf5pg</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Essie French Manicure and some cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itf5pg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1itf1ep</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Cityscape is like a party on the nails</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pn70xz6ej5ke1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1itez52</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>The beautiful ILNP flower child deserves its popularity</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itez52</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1itdoz9</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Nails inspired by driving in the snow!</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itdoz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1itdlyc</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>BKL Mystery 🔎🕵️‍♀️</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itdlyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1itcyzq</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Beneath the Surface</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itcyzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1itc5bs</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Matching my polish to my engagement ring</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itc5bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1itbphn</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>A beige base with a gold glimmer of hope to match my at-work mood.</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itbphn</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1itb2b0</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Horn of Healing by Arcana Lacquer 💅✨</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itb2b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1itadu1</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>5 Color Skittle, Spring/Regency Inspired</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itadu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1it9srb</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>First try at butterfly nails! My hand's still shaking</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it9srb</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1it9qq2</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>🧡🩵Wicked Sweater🩵🧡</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it9qq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1it9fz0</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>[ISO] “Doomsday” Fish Colour</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzvdd3abg4ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1it7ufv</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Got a paper cut on my finger. My thermal nail polish changed colors</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/is8tlbwl44ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1it7r35</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>My experience with Glisten and Glow vs Seche Vite</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1it7r35/my_experience_with_glisten_and_glow_vs_seche_vite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1it7k3k</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Peeps polish</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p748qne24ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1it7i0s</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>New detail brush = nail art!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it7i0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1it7cr5</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Best Luxury Polish?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1it7cr5/best_luxury_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1it6nz5</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>My first polish from PPU. “Under The Guise of the Moon &amp; Stars - PPU J25” by Dany Vianna.</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it6nz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1it5ej0</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Colores de Carol</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it5ej0</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1it56eg</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>My way of dealing with tip wear (imperfect I know)</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aspjb4gi3ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1it2ji9</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>A jewel beetle using Jewel Beetle 🪲</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it2ji9</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1it1g5r</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it1g5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1it0xsv</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Please help!! Best sponges for gradients?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it0xsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1its07r</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Help me find a good nail lamp</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1its07r/help_me_find_a_good_nail_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1itpk7k</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>one of my all time favorite pedis omg</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itpk7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1itoand</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9xm30iqk7ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1itnbew</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts Nobody &amp; Sea Salt Ice Cream as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itnbew</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1itn1tw</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>My Best Valentines Nails Yet!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztsz399p97ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1itmt05</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Violet and pink nail art</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am50uouh77ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1itmq6x</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Just started</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itmq6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1itl86x</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Umaru-chan hand painted nails 💅🧡</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g47r2od7u6ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1itksqu</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>feels like I've regressed</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q75mnadoq6ke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1itks8a</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Please help!! Best sponges for gradients? Info below</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itks8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1itjp3b</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Princess Mononoke hand painted</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cpbruxosh6ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1itjmh9</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>This set EATS LITERALLY 🫦</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x4dmk9t7h6ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1itjj31</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Junji ito press on nails hand painted (tomie💕)</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itjj31</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1itexmz</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>love nails</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ks2677sii5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1ithwg9</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Another vday look</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5tj77sb46ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1itf1rp</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>did these on vday and fell in love 💜</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjz3gdgij5ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1itbrnd</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>How cute are these LV inspired nails , these were done for me by @vst_exclusive_spasalon fully hand painted I’m in love</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1lzud7khw4ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1itbj0w</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Honduran food 🩵</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itbj0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1itarx8</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Fairyland nails 🧚🏻‍♂️</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itarx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1it9ins</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>This was my second set ever, I think or my third, black, gray and red vampy stilletos</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it9ins</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1it8bs0</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>How to bend glitter/sequins down to curve nail</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1it8bs0/how_to_bend_glittersequins_down_to_curve_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1it7m4p</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Cat Ear Nails</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wqok5bms24ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1it79t3</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Total newbie</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it79t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1it5gcs</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>this is my fav set i’ve done 🥹</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it5gcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1it4bpw</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>A Chopin-inspired press on set 🎶</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it4bpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1it3kdg</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Nail art realizado a mano alzada a una clienta en mi salón temática “catrina”</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it3kdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1it1wj8</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>new nails🍒🌈💕</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1it1wj8</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Feb 21 08:10:50 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_23.xlsx
+++ b/data/collected_data/2025_02_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C862"/>
+  <dimension ref="A1:C1056"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15087,6 +15087,3304 @@
         </is>
       </c>
     </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1iult8y</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>BIAB is a godsend for nail biters</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iult8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1iulm96</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iulm96</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1iulhb9</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>5 hours later...</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iulhb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1iulf6o</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Hii! I have a question about temporary nail glue solutions!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iulf6o/hii_i_have_a_question_about_temporary_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1iuknuv</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Best nail kit for beginners</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuknuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1iukp5m</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Thoughts on this set I just did?</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8ruv30tufke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1iujtpn</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>First time doing mid century nails 💅</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iujtpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1iuiw83</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Do my nails grow fast or am I being scammed</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuhk5r88bfke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1iuj32s</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Need ideas for my next mani</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6o7ldd3dfke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1iuiu28</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>new nails!</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dirce6mafke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1iuim7t</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Measuring Press-On</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iuim7t/measuring_presson/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1iuik4r</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>help with nail cost?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvt477fr7fke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1iuihht</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Kuromi Nails 🎀</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxvxcea37fke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1iui3md</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Acrylic took off real nail</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iui3md/acrylic_took_off_real_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1iui33z</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>coquette lilac 💜🎀</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iui33z</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1iui0gq</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>epic plaid nails ✨</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iui0gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1iuhwp6</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Love this color</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/448l3c2g1fke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1iuhsio</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>How do my natural nails look?</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuhsio</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1iuhq41</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuhq41</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1iuhcd4</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Gorgeous nails I got for my bday are a little too small</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lkn6jjzveke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1iug9s1</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Will be kissing this set bye on Sunday</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpkbu4f5meke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1iug5u4</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>✨️INSPO✨️</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iug5u4/inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1iugybm</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Static Pressons question!</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iugybm/static_pressons_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1iugwnb</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Got my first manicure ever today 💕</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0jtzcuwreke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1iugudl</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Not sure what to title this</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biipzipbreke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1iuggtg</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>First time using acrylic</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrpkebyxneke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1iug6rt</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>gel polish question</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iug6rt/gel_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1iug5dt</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Do these look like press ons?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iug5dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1iug17r</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Que horror</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iug17r</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1iufz98</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>I love my new nails</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iufz98</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1iufsb9</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>A little French, a little floral.</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0duagxpvheke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1iufp69</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iufp69/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1iuflgj</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>GenesisTheGawd gets her nails done</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ew41kxd8geke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1iufkk6</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Anniversary nails that my fiancé picked 🖤</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrc5eot0geke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1iuespu</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>your opinion</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tzc6stdb9eke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1iueocb</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>$25 set</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4ynwyx98eke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1iuejyy</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>First time trying out this shape versus my usual!</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuejyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1iudgw9</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>How to deal with Fire Rings (help please) 🙏🏻😪</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iudgw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1iud6a2</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>I painted press ons for my sister! This is traditional lacquer on gel extensions.</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iud6a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1iudaz3</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Espresso Martini Nails!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ov5orrh7udke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1iud0y5</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>First time using nail charms</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iud0y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1iucrle</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Cateye nails that don't need cured?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iucrle/cateye_nails_that_dont_need_cured/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1iucqv7</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>What’s your go to?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iucqv7/whats_your_go_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1iucjns</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Grow Out?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iucjns</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1iucj8p</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>1st set of acrylics,not my fav</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mm6590xndke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1iuchi4</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>2nd set of acrylics I ateee,I did cherries nd glitter bottoms!</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuchi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1iucgmw</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>I'm still struggling with the chrome on the cuticle area, but I like them 💕</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iucgmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1iubxvc</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Press ons question</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iubxvc/press_ons_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1iuc5tw</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Advice please: bubbly/bumpy polish right after appt</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iuc5tw/advice_please_bubblybumpy_polish_right_after_appt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1iuc0v2</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Tried a new shape, do they work?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuc0v2</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1iubwut</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Hard Gel</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iubwut</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1iubrx6</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Broken Nail Help</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iubrx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1iubrbo</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>which shape?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iubrbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1iub3v5</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Out of this world?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n1wktr1pcdke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1iubkpq</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Does this shape look okay on me? It's hard for me to tell.</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnfugi1agdke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1iubjrq</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Addicted by rougenoir</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iubjrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1iubi6t</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Am I about to kinkshame a nail polish? 🤔</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ira31zrjfdke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1iubez5</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Gfs nails 😍</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/64o582w1fdke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1iuacrn</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>My work. What do you think?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuacrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1iub5h2</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>I was fascinated</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9if5f01ddke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1iub4hv</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Lillies for my daughter Lily’s birthday</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iub4hv</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1iuaywq</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>My Birthday Nails! 🧸🤎</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nva3g6cnbdke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1iuasw8</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>😈🖤</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w8bz8feadke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1iuap1s</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Which nail shape fits my hands best?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuap1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1iua6xf</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Hard gel vs. dip</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iua6xf/hard_gel_vs_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1iua195</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Couldn't decide between French and plain red 🙈</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mjhpbkn4dke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1iu9tc7</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Same light for both?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iu9tc7/same_light_for_both/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1iu9ld8</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2m7pwqye1dke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1iu8xqq</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Gel nail help! Complete beginner</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iu8xqq/gel_nail_help_complete_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1iu8d0w</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>what do you think about piercing on nails?💫</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu8d0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1iu7yv3</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>same vacay set but this time done with my non dominant hand🌴🍹🌺</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9okhkecpcke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1iu74y7</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>1 Year Nail Care Progress</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu74y7</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1iu7gc1</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Run to Micheal’s !</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sio0yt1llcke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1iu78rk</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Proud of this set 😤</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu78rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1iu72qc</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Cat eye, chrome, and rose foils</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu72qc</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1iu6n20</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>The lady who does these charges me the equivalent of 18 USD and I feel like I’m robbing her</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu6n20</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1iu6h2f</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>I loved this design!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkcfxzukecke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1iu6grj</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Barbie Sunset Malibu PJ set</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu6grj</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1iu6arc</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Can you mix UV and LED gel polishes?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iu6arc/can_you_mix_uv_and_led_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1iu62v0</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>This set I did today... just YES</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ll7p5cpbcke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1iu629e</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Little bit late for Valentine’s Day but… what the heck lol</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uh0d5elbcke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1iu5sb9</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Just finished these, super proud of them 🥹</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu5sb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1iu5pfs</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Acrylic Overlay</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iu5pfs/acrylic_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1iu4udm</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Woman Owned Nail Business</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iu4udm/woman_owned_nail_business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1iu5qkm</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>I painted the queen of the hour 💙</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wx5e9ln79cke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1iu5141</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Juicy &amp; frozen in WI rn</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu5141</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1iu4ywz</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Found a new place. Happy 🍓🐾</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu4ywz</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1iu4o2z</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Valentine's 2025</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu4o2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1iu4k11</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>I think it's the cutest design they've made for me so far. What do you think?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu4k11</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1iu3srq</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Lifting gel at free edge</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iu3srq/lifting_gel_at_free_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1iu3wd1</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>What to get for “spa-ish” mani/pedi care?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iu3wd1/what_to_get_for_spaish_manipedi_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1iu3w7a</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Dry Nails?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu3w7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1iu3qyi</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Almond nails</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zp2lox41vbke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1iu3ifh</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>My first Russian manicure</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0wthpodtbke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1iu339y</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Before and after</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu339y</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1iu31nu</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>New nail day</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu8pz3g2qbke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1iu2idi</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Ive been trying to level up my nail game</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu2idi</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1iu2dlc</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Phoenix - Oops #20</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu2dlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1iu1oht</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>First post! Did these myself. Anyone else has nails that grow in different shapes? My pointer and thumb grow round and my other ones grow square</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu1oht</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1itw34b</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Best way to remove gel x extensions?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1itw34b/best_way_to_remove_gel_x_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1iulsae</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>I've renamed this one Punch-you-in-the-eyeball Pink 🤣</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iulsae</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1iujfx1</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>First magnetic polish</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/taxr8ktrgfke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1iuites</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Talk me out of this, talk me into this, tell me what I should get instead? First ILNP order overwhelm &amp; my lizard brain that loves pink/orange shimmer is taking the reins</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c92l5qlfafke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1iuicp0</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>What are you getting from the BLK sale tomorrow?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpbmuwoq5fke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1iui40g</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>The husband and I are still feeling the wintery blues ❄️</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyayn8nd3fke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1iuhohq</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Velvet attempts #1!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuhohq</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1iuh8jf</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Recommendations for a thin formula, high-shine top coat?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iuh8jf/recommendations_for_a_thin_formula_highshine_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1iugv7k</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>In LOVE with this Sally Hansen polish</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iugv7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1iug8rk</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>It's giving 2019 Eilish vibes and I *love* it</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iug8rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1iug647</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>L.A. Colors Jelly!🤎</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iug647</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1iug5i8</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Zero Degrees in the snow 🌨️</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iug5i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1iug5he</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Salon did not properly cure my gel manicure - what steps can I take now?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iug5he/salon_did_not_properly_cure_my_gel_manicure_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1iufujc</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Requesting product recommendations</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iufujc/requesting_product_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1iufa34</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>I can't decide which version I like more</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iufa34</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1iuf9dt</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Help?!?!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iuf9dt/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1iueuzy</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Mooncat Match Made in Heaven</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gcdkn74v9eke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1iuetxc</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Lurid, the Wisdom of Your Armor</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuetxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1iudndu</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Fluid art tips?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iudndu/fluid_art_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1iudlma</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Anyone else guilty of neglecting their minis?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvi4h5elwdke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1iucjv3</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Proximal nail fold vs cuticle?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yi8olms1odke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1iuc3sp</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Am I about to kinkshame a nail polish? 🤔</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0hv4sfc7kdke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1iubzhc</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>What have you learned about yourself/preferences since starting your nail journey?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iubzhc/what_have_you_learned_about_yourselfpreferences/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1iubyf4</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Does anyone recognize this polish by name?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/th8brkpajdke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1iubl9e</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>GLL Great Balls of Ice in that evening golden hour</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnlhal6egdke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1iubhu6</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>SNS Removal post 5 years</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gllome8ofdke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1iubafl</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>I did It again... Rougenoir</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iubafl</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1iub6o1</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Linear holos- faves?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iub6o1/linear_holos_faves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1iub413</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>I present to you... "SHURPLE!" The worse case of ugly bottle syndrome I've ever seen.</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iub413</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1iu9qfg</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Galaxy vibes</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/criou1vf2dke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1iu9k7w</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Thermal swirls</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu9k7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1iu9i6g</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Mooncat - Firewall</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/twxjlevb0dke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1iu9gcm</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Dupe Recommendations for MN Polish - The Sword?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu9gcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1iu8qu1</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Icy snow day mani ❄️</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu8qu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1iu8mab</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Clionadh surprise!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu8mab</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1itzifq</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>My nails hurt a little when i press them after taking off my press on nails</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1itzifq/my_nails_hurt_a_little_when_i_press_them_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1iu2nba</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iu2nba/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1iu2v37</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Black diamond, red nails combo just hits.</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uht54t6robke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1iu7hpl</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Curious about Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iu7hpl/curious_about_death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1iu7cv0</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>“Aries - Rainbow Obsidian” from the Zodiac Stones Collaboration between Dany Vianna, Vanessa Molina, &amp; Whatcha. Shown in 3 coats. 💖</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu7cv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1iu7bup</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>New Cursed Thumb Pose Unlocked</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu7bup</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1iu76t4</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Matching my lady with Root of all Evil by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbh9njjojcke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1iu75at</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Swatches of LAColors jellies!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu75at</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1iu71yq</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer "Fire and Ice"</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4ewmrloicke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1iu6nq8</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Eastern MA folks - FB storage find</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iu6nq8/eastern_ma_folks_fb_storage_find/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1iu6i6i</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>The glow!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iu6i6i/the_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1iu6h45</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Aspen by ILNP</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu6h45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1iu6daz</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>A Galaxy Far, Far Away</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzi1y9ppdcke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1iu63ct</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Blue or Purple? Blurple?!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu63ct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1iu5k2a</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Recommendations for drugstore nail polish brands in Europe?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iu5k2a/recommendations_for_drugstore_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1iu5cur</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Mooncat +Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu5cur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1iu3vt0</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Turquoise recommendations</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iu3vt0/turquoise_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1iu3p1v</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Banquet of Breadcrumbs is so unique</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5k1y59oubke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1iu30px</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>My mechanic likes flower child too 😛</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqkrkuawpbke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1iu2e3a</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Phoenix - Oops #20</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu2e3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1iu29gl</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>That gas station lighting is *chef's kiss*</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwxq1yjakbke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1iu1qr2</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Photos don't do it justice so here's a video :)</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xzlinrh8gbke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1iu11pv</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Shaping Help</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iu11pv/shaping_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1iu0qsj</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Freefall</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu0qsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1iu06rn</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Eucerin lotion gums up my manicure. Every. Time. Has anyone else had this happen?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iu06rn/eucerin_lotion_gums_up_my_manicure_every_time_has/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1itzo6g</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Atomic Polish Juniper</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itzo6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1itzc9n</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Anyone else like doing their nails on vacation? 🥰</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itzc9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1itz5c1</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Purple skittle in different lighting💜☀️📸💡</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itz5c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1itz3l2</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>cat tax included ➡️</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itz3l2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1itz3cf</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>First time using soft gel tips - I think I'm hooked</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itz3cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1itwxoq</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>TBCA... what is it?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1itwxoq/tbca_what_is_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1itw72n</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Can anybody help a colourblind girl out? 😅</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm0aim9o2ake1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1it5ltm</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>In love with this neutral</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcd2tqhfm3ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1itc7fb</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>New favourite trend: random skittles</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itc7fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1itlvq8</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>One year progress of doing Russian nails and I can’t believe my nails grow this long .</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gztpgbhnz6ke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1itveba</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>🧿🧿🧿</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpq3j80xs9ke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1iulgrl</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Porcelain Simpson Nails?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ptcvuig4gke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1iuakex</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Top coat (gel) still sticky after curing and wiping with alcohol</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iuakex/top_coat_gel_still_sticky_after_curing_and_wiping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1iujvi0</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Kitty Nails</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/859riupdlfke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1iugusk</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Design</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2dlq4hfreke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1iuf6x9</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Snake Nails</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuf6x9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1iudkra</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Sweethearts set 💝♥️</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iudkra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1iud289</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Hey y'all, I'm looking for feedback on some of these designs I've made. Are they too boring, not really in style, or do you actually like them lol? Please let me know!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iud289</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1iu9b52</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>My first time using blooming gel! :)</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu9b52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1iu8roc</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>To those who do Anime or more detailed Nail Art: How long do you take?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu8roc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1iu7lc1</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Early 2000’s baby here</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu7lc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1iu7kwe</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Was inspired by the souvenir (a mirror) my colleague gifted me on her holiday in 🇲🇦</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5t7spdkkmcke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1iu6qsz</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Inspo and product testing accounts</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iu6qsz/inspo_and_product_testing_accounts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1iu6iat</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Barbie Sunset Malibu PJ set</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu6iat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1iu4nuu</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Just got nail stickers for the first time!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rnv5jyi1cke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1iu4sxh</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Brushes</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwjyq27m2cke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1iu4g59</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>I love sharks 🦈 (valentines design on nails)</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjorydy20cke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1iu29yk</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>First time wearing milky white chrome frenchies ✨</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu29yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1iu1gth</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Wanted to share my Valentine nails before I paint a new set 🥰♥️✨</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu1gth</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1iu0uct</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Little late but I finally did some valentines nails 💖</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iu0uct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1itybhj</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Anyone know roughly how much these would cost in £? (Oliviarwallace on Pinterest)</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6q7bfveooake1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1itx7sm</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Bridgerton Vibes :)</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxjfwek0eake1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ituttd</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Nail Art</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ituttd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1itvbdv</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>My new set of nails!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1itvbdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ittm7m</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Sanrio nails I’ve done</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ittm7m</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Feb 22 08:09:21 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_23.xlsx
+++ b/data/collected_data/2025_02_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1056"/>
+  <dimension ref="A1:C1246"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18385,6 +18385,3236 @@
         </is>
       </c>
     </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ivc0us</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Why did my ombré acrylic manicure turn out like this??</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivc0us</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ivbv0a</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>I’m getting better.</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivbv0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ivbt1j</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Best nail shape advice?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivbt1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1ivbp0f</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Happy Friday ✨</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/208q2kc0omke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1ivbitw</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Best light with fan</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivbitw/best_light_with_fan/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ivbg08</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>First time nail art, tried thebhungry caterpillar</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdzc0uz8lmke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ivbbel</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time today and I don’t know if I’m just being overly critical</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivbbel</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ivb7oo</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Manifesting Spring 🌱🌸💅🏻</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivb7oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1iv9td5</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>I neeeeee to know if these are good or bad.</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va32u5de4mke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1iv832t</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Does anyone know what nail polish she’s using here or how else I could get this effect at home? Credit to @kmxnaildiaries_ on insta.</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv832t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1iv8bhu</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Wanted Lavender and Got Pink</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pjb557yplke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1iv9xp7</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Do these look like $1 nails?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9tku5wl5mke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1iv9twq</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Wild cat print nails!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv9twq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1iv969t</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>I received compliments on my nails today 😊</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pihw38q0ylke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1iv8ol4</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Brittle ass weak ass nails</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iv8ol4/brittle_ass_weak_ass_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1iv8pn1</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>I made these two sets today, what do you think? My girls are risky with their designs 🫣😍🌸🍒.  Set 1: $27 set 2: $25</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv8pn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1iv8mvf</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Playing with my chrome powders🦄🌈</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23143qywslke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1iv8mkd</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Monopoly Man!</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kppab13uslke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1iv8j3d</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>First at home dip manicure attempt</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpgm1hrxrlke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1iv8e1f</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Question about Chrome</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iv8e1f/question_about_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1iv8d2p</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>My first ever wedding set!!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv8d2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1iv8cxp</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Wow 🥹😍😱</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chorntebqlke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1iv82cp</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>freestyle set 🫧</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv82cp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1iv814x</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Freestyles are my favorite</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv814x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1iv7x3e</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Advice on color and shape of French tips</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv7x3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1iv7lsh</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Any nail techs? Advice please</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv7lsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1iv7smk</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>White Polish + Matte Finish = Yellowish Nails?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlkj3dm6llke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1iv7ezm</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>marble 🖤🤍🩶</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avys184uhlke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1iv71hq</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>✨Grounded ✨</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtma5l6felke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1iv6oun</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>I do my own nails and this is my favorite set so far!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq7ajjy68lke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1iv6llm</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>3 Weeks. Awesome.</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv6llm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1iv5mze</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Growing mm by mm</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv5mze</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1iv5m8i</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>I told my nail tech to do whatever and she didn't disappoint.</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv5m8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1iv5ima</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Something new</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv5ima</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1iv5an0</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Tell me honest 😭</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv5an0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1iv58ni</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Chrome question</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbwnivzyvkke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1iv50zr</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Did I get scammed? Cat Eye Nails</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv50zr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1iv4twj</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>2 week nail growth 🙌🏻</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv4twj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1iv4clw</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>My Current Nails</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv4clw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1iv4412</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>baby pink cat eyes 🩷</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv4412</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1iv35bi</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>I &lt;3 my Nail Tech!</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97we9wshfkke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1iv2wxy</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Going short this week💅💅</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sj8o8otrdkke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1iv2p8n</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>I listened! 😌</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv2p8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1iv2g3g</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>I feel like a princess 👑</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv2g3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1iv25zc</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>No longer a nail biter!! Last August, i decided that at almost 49yr old, it was time to quit biting my nails. I'd tried many times over the years and always failed. I found a nail tech that was up for a challenge in helping me stop. She used BIAB and for the 1st time, i have proper nails!</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv25zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1iv1rcs</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>What are the best SNS at-home recommendations?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iv1rcs/what_are_the_best_sns_athome_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1iv1h8d</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Isopropyl alcohol (IPA 99%)</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qelqxc13kke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1iv1qz6</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Never tried blue before, what do y’all think?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv1qz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1iv1fg7</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Fox and the Hound nails 🦊 🐶</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aw3u7w6o2kke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1iv17fd</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Does this shape look ok on me?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv17fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1iv11kc</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Which nail is your fav?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kk8xu4wszjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1iv0rly</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Natural nails with only garlic shine and cleaning every 10 days 😍😍😍 (I like to take care of my clients' nails) 😍🥰</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8ueb1zqxjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1iv0oq4</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>We’re manifesting ✨spring✨💛</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv0oq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1iv0igi</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Gel polish lifted and did this to my nail, any tips for how to recover my natural nail?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0dfd6zksvjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1iv0fpd</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>How to make sure longer nails don’t break?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qksp8zu7vjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1iv09mo</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>My first nail sets I’ve created</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv09mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1iuzllh</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Should I cute the excess bits on my cuticles, or do they just need to be moisturized?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuzllh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1iuzgo9</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Which shape looks better?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuzgo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1iuzemf</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>I forgot to cut My nails for a 2 weeks</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuzemf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1iuz7vi</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>My best friend and I decided to get the same design.</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgil5x94mjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1iuyznu</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Burgundy and navy blue = underrated combo</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/874jfligkjke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1iuxwn4</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlnwyudkcjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1iuo3e4</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Onycholysis</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iuo3e4/onycholysis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1iup7yz</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Want some input from those who wear nails and work with your hands.</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iup7yz/want_some_input_from_those_who_wear_nails_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1iutug0</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>My nails are killing me. What can i do?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h19b2faziike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1iuwt5k</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Got this done for approx $32 in my country</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuwt5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1iux8nn</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Why does builder gek never work on me?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3pjnq4r7jke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1iuwsze</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Custom🩵SouthWest🩵press ons</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iurbamkm4jke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1iuwo70</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>I loved them! The manicure made a very beautiful</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuwo70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1iuwbdb</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>some of my fave nails i’ve had</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xn004c71jke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1iuw8n6</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>white nye set</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/296tczfn0jke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1iuw1la</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>$30 set. Do the girls really like these designs? 😍😍</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lio2z5w7zike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1iuw15d</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>my hello kitty nails ♡</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xaqt00s4zike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1iuvklw</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I did it!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0awsmwuvike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1iuvg1l</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qnsmpexuike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1iulwq1</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Nail inspo for anybody</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iulwq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1iuu298</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Vegas nails ♠️</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuu298</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1iutrqx</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Shamrock shake inspired- idk if I like them!</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iutrqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1iuuy32</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>My cuticles are not the best but love the design 🩷✨</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzzriec8rike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1iuuw86</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>wanted to show off my natural, painted nails!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuuw86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1iuuw5x</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Measuring Press-On</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iuuw5x/measuring_presson/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1iuundn</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>It was hard making longer nails look like strawberries</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e8lxu40pike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1iuuiup</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Soap Nails: What nail color to use?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iuuiup/soap_nails_what_nail_color_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1iuudoe</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iuudoe/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1iuu6a6</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>black French pedi 🖤</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqisdomilike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1iuu1ez</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>French tips 🤍</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuu1ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1iutw34</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>My nail lady is amaze-balls</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iutw34</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1iuthtp</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Me cobraron 20 usd por estas uñas me parecen que están baratas que creen</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu46h1yagike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ius9ej</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>February nails 🍒🩵</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ius9ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ius1p7</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Wishing for springtime</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zeq5xavt4ike1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1iuroyd</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>First time doing gel extensions</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuroyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1iur8da</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Omg i love them 🩷</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/521it2w1yhke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1iuqmxg</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>any hope with genetically weak nails?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iuqmxg/any_hope_with_genetically_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1iuqjne</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me? I have been doing almond but want to know if coffin/ square would look better</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuqjne</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1iuqgcj</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>pink and pretty 🩷</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuqgcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1iuphjs</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I changed up the shape again with these deep red cat eye nails. Not sure what my favorite is yet.</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxklbrpqhhke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1iup9xm</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Got my nails done today and didn't get to ask what shade they used, what's a drugstore (non-gel) dupe of this color I can look for so I can do them on my own at home?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65yn0jflfhke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1iup917</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>New nail color</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iup917</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1iup78f</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Most perfect nails💙🤎</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iup78f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1iup3kf</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Birthday nail set 🩷🎂</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyfbvscrdhke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ivdcw6</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>February Amethysts 💜</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0ltiupe7nke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ivcdf8</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>told the northern lights to keep shining ✨</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/01wv9jwpvmke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1ivc2tp</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Shiny Milk Chocolate!</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivc2tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1ivbxfn</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Can anyone tell me the polish they used or how to get this effect at home??</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivbxfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1ivbi4d</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>How often does Cirque do restocks?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ivbi4d/how_often_does_cirque_do_restocks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ivb7wi</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Blue to teal or green multi chrome?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ivb7wi/blue_to_teal_or_green_multi_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ivau7s</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>moar moar magnetics</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66l4kk8qemke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ivap6r</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Supernova sunset</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivap6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1ivab2j</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>The first EdM lacquer I’ve ever tried, absolutely obsessed</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivab2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1iv7nnc</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>oh hi, magnetic mashup</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv7nnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1iv6v56</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I don’t pain my nails often but this sub has been inspiring me! I tried to make a jelly polish with products I already had.</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv6v56</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1iv6jb0</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Which company sells the best one coat black polish?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iv6jb0/which_company_sells_the_best_one_coat_black_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1iv6gzf</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Decided to mix two icons</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4rsgpmu86lke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1iv5z8d</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>My most complimented polish. It's like wearing butterfly wings 🦋</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv5z8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1iv54u6</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Andromeda is out of this world</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv54u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1iv4sqc</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Lavender with a subtle grey pearl sheen</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv4sqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1iv4dyl</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>So pretty!</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv4dyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1iv45hn</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>One polish 4 colors</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv45hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1iv3wei</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>This but just the Shimmer?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrlhimjclkke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1iv2cks</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>LA Colors has no business being as good as it is for how cheap it is</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv2cks</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1iv23yt</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>New favorite thermal feat. my dog who needed to be the center of attention.</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv23yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1iv22z0</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Glowy shorties</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv22z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1iv20vp</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer — This is Where I Thrash</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv20vp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1iv1vfi</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Lifestream</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv1vfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1iv1gec</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>When organizing do you keep  PPU/HHC/LBOH polish in their own group?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iv1gec/when_organizing_do_you_keep_ppuhhclboh_polish_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1iv1385</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>slightly damaged top layer of nail - what should I do for it?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1do4km050kke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1iv134x</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Palm Royale Nails!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t40t1f40kke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1iv0v1s</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Took some of the cuticle and PNF care advice I asked for yesterday and I feel like I see a difference already!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ldethy9yjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1iuztnp</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>forbidden fruit is barista approved ✨</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4gg0ixfkjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1iuzmhn</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Should I cute the excess bits on my cuticles, or do they just need to be moisturized?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuzllh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1iuzji1</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Twilight Tea Party at a garden party</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuzji1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1iuyszn</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>✨️🌈Neon Gradient🌈✨️</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuyszn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1iuyk5x</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Emily de Molly "Such A Farce"</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3mnhbkahjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1iuyhin</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Cupcake polish brushes</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iuyhin/cupcake_polish_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1iuy0iu</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Dracula: an A England favorite</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/940sb3eadjke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1iuxq9u</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Steep Dreams 🌌</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ae3u0i4abjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1iuxgsy</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>On day 9 of my manicure!</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuxgsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1iux858</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Was not intentional but definitely looks like a mix of belated Lunar New Year and Valentine's nails.</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtnfp7h37jke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1iuvvjp</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Starry eyed - without stars 😩</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuvvjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1iuvtpe</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>pahlish - mushu 🐉🌶️</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuvtpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1iuvlf9</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>So have we found a basecoat that doesn’t cause peeling?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iuvlf9/so_have_we_found_a_basecoat_that_doesnt_cause/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1iuv99q</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Seche vite with KB Shimmer thinner?</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iuv99q/seche_vite_with_kb_shimmer_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1iuv16w</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Finally got my hands on jelly polish</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9lnu0evrike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1iuus88</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Zoya Corinna and Patrice on brown skin</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuus88</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1iuus3w</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Oh BKL Lemon is breathtaking 🥰🍋</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuus3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1iuupbk</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>emotional support taco 💚🩵</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuupbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1iuup39</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>The Butterfly Effect</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuup39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1iuulub</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Shifty purple</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7r78upooike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1iutja6</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Cirque Colors chiffon</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iutja6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1iuteea</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Little rainbow sunsets</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gswm3a5efike1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1iut93n</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Does Sassy Sauce do sales outside of Black Friday?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iut93n/does_sassy_sauce_do_sales_outside_of_black_friday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1iusl0i</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Blue drugstore polish skittles!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iusl0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1ius3at</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Wishing for spring</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1obmti965ike1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ius1un</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>How do I use this nail recovery treatment?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7rjcunu4ike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1iurky8</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>ILNP Spoilers for the Feb 28th Collection</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vkxr2f111ike1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1iupps9</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>ISO la reveuse chanel dupe?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5899ec0khke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1iupbvw</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Long time since I got my nails done</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iupbvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1iuoyw3</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>ISO yellow and pink thermal</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgifarlbchke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1iuosoe</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>A holo pearl-white, created with the powers of layering</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuosoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1iuoig5</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Fell in love with Essies shade Mezmerised 💙</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jxl68c17hke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1iuobts</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Any tips for nail health?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iuobts/any_tips_for_nail_health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1iufkz3</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Nail Rings - recommendations?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iufkz3/nail_rings_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1iv70jo</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Anime Nail Art</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcypdb87elke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1ivarya</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>How was the nail design?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s04s53t6emke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ivcw02</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Playing with Icegel sunset chromes🌈🦄</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j7br3ust1nke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1iv9sda</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Wild cat print!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv9sda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1iv9exn</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>I love them!!❣️</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiwf1kze0mke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1iv98aa</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>My Mama Did Them!</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1alihykylke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1iv8r0p</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Be honest with me do these nails look bad</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv8r0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1iv8py4</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>pink set :)</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56gel44qtlke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1iv8g17</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>I'm just getting into doing my own nails; this is the first nail art I've tried:3</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv8g17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1iv6u9b</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Evil eye set</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rc8u52mclke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1iv5ogr</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>keep practicing and experimenting with cat eye</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76kyu6umzkke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1iv5mez</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>first attempt at cateye, took a solid 10mins to figure out the magnet 😅</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fskatvn5zkke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1iv4hul</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Hearts or Spookies</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y82kq48wpkke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1iv42a2</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>My very first set on a human 🥰</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv42a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1iv2ih8</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Feelin princessy 👑</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv2ih8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1iv1eu0</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>I love clear nails 🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iv1eu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1iv0f30</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>I'm in love with this result!</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmooeyyxujke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1iuzxf3</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Favorite set of the week</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuzxf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1iuzrvb</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>I still have a lot to improve, but here’s my first attempt. Give me some tips!</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0grpq27qjke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1iuvgpq</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>my NYE set still hits</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rfdv4gp2vike1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1iuusa9</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>hey girls 💖what you think about my Valentine’s nails?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk97etn0qike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1iuuqn5</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>These came out so cute I can’t stand it</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7rwryeopike1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1iuou6a</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/riyzurktahke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1iuquhj</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Favorite set I’ve made so far</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iuquhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1iuqbot</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Late Valentines nails 💖</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnrd9mdzphke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1iuped8</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Meadow :)</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1i8t04cughke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1iumuzd</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>DabDaDan nails Hand Painted</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u90prxxfmgke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1iumtgc</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Junji ito nails hand painted ✨</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iumtgc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Feb 23 08:09:30 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_23.xlsx
+++ b/data/collected_data/2025_02_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1246"/>
+  <dimension ref="A1:C1424"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21615,6 +21615,3032 @@
         </is>
       </c>
     </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1iw5a6l</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Trying out new colours for my new era</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw5a6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1iw58we</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Is it safe to keep these BIAB nails for another 1,5 weeks?</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw58we</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1iw58hr</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>My first attempt at acrylics</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw58hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1iw57lb</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Nails for school auction</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zzyii1piuke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1iw4oaw</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I miss this look</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25ck1kzxbuke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1iw4jv4</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>obsessed with my manicure today</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uz4oyzoaauke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1iw47on</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>It's gone</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw47on</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1iw3es1</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>medieval nails</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw3es1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1iw3sxy</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l8u2wzeb1uke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1iw36yw</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Do u think I like Hello Kitty?🖤🩷</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8h2m6t99utke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1iw32jm</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Baby blues 🩵☁️🩵☁️🩵</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l93zu0xvstke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1iw2ywf</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Recent nails</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw2ywf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1iw2w0l</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>My very first set!!! I know my cuticle prep needs work lol😭 what do we think? I free handed the frenchies so they aren’t 100% perfect</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw2w0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1iw2qzf</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>I actually really like this color and i do my nails by myself cause im to broke to get them done, eventually in the summer ill do designs but bc of school i cant, anyways what do you think:)</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d78oukcptke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1iw2na1</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Pedicure sanding</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iw2na1/pedicure_sanding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1iw265i</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>can never go wrong with a baby pink</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7pycpu6jtke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1iw23pz</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>✨Ethereal Vibes All 2025✨ -Dip powder on my natural nails.</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw23pz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1iw1vx2</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>1st Builder Gel (in a bottle) attempt!</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw1vx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1iw1kf2</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>🍭🍭🍭 needed some color!</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yubiqzhwctke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1iw1jgt</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>beautiful design</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o77iylnctke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1iw1fjh</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>What do you think of this style of French nails with gold?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw1fjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1iw1cea</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>My tech NAILED it!</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r5mspxratke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1iw0qd4</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>What’s my nail shape?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktjoempp4tke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1iw0ij0</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vh0oguqj2tke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1iw0ieg</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>My wife nails</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw0ieg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1ivzjjw</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Before and After Mani</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivzjjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1ivwfnl</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>my nail is super sensitive to cold after regrowth !</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivwfnl/my_nail_is_super_sensitive_to_cold_after_regrowth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1ivwhd0</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Are these bad?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivwhd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1ivzlod</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Advice needed</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzali9trtske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1ivzlh2</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Freaking love my nails!</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivzlh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1ivzkc3</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Nail Polish Dupe</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivzkc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1ivzj78</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>My last 2 sets (Gel X)</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivzj78</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1ivz3ht</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>polygel or biab</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivz3ht/polygel_or_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ivyrfg</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>My nail tech is amazing😭🖤</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sf5b11xxlske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1ivyqoz</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>My first time with builder gel + cat eye</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivyqoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ivyjj2</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>thoughts on Polygel technique? This is my third time practicing on filling in natural nails</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xxm3ewwjske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ivy8q4</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Round or square ?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivy8q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1ivxywr</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>My sister did my nails a while ago nonbinary flag on the left trans flag on the right</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ubv0t7peske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1ivxrzd</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>froot 🍋🍒🍓🥝</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivxrzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1ivxrqa</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>needed a pick me up</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivxrqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ivxkb3</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>These help me from biting my nails</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivxkb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ivxi33</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>I call them my beetle nails</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivxi33</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1ivx9d0</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>wishing for warmer days 🧡☀️</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0i8pole8ske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ivx3a6</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Living my best Hello Kitty Island Princess life</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivx3a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ivwyaw</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>🩶✨silver &gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivwyaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ivwxah</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Some French tips I did on myself</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oobbztli5ske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ivwm3g</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>How can I regrow this nail? (Not a nail-biter)</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjwqyfnr2ske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ivwh7y</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>I might be (just a tiny bit) obsessed with this pink 🍭🩷</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivwh7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1ivvzhi</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Super simple but I think they are cute</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aefe30dexrke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1ivuc0u</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Fishing lure nails!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivuc0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1ivvl0u</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>🧚 ✨ 🍄</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sg9649ztrke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1ivvi54</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Birthday nails🥰</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivvi54</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1ivv88x</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Gel Polish Change</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivv88x/gel_polish_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1ivuwzs</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>My December nails that I loved so much 🍷✨️</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ip3k2gweorke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1ivum16</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>starting out</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivum16/starting_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1ivufnr</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>jade-ish?? first attempt at a polished stone effect</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivufnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1ivu9j2</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Not bad for press on’s!</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyf5jdv4jrke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1ivtzno</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivtzno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1ivtr0x</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>new favorite shade ✨</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivtr0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1ivtnkk</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>My nails are longer than my patience 😂💅🏼</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgb14nk5erke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1ivt9ge</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Beginner nails!</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivt9ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1ivt8sv</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Messing around and slayed these !</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xag5nvnwarke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1ivt38e</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>How did these turn out</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euax9iln9rke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1ivt349</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Ever since I got engaged/married, I quit biting my nails. I feel like I have accomplished a goal I have had pretty much my whole life 🥹</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivt349</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1ivstw8</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Looking for Tips for Dashing Diva Glaze or Ohora especially for stronger nails and longevity</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivstw8/looking_for_tips_for_dashing_diva_glaze_or_ohora/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1ivsr1t</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Beam us up, Mr. Scott!</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivsr1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ivsgxh</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Just did my nails for the first time and I got cat claw nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivsgxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ivs849</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Happy with how these jade stone nails turned out</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfv8tkjv2rke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ivq33u</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Beginner Nail Lamp</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivq33u/beginner_nail_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1ivr4va</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>french tip base color suggestions</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivr4va</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1ivr5pv</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Went with animal print this time</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yzxi8aguqke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1ivqze7</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Natural nails/Ombre😍</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3omezr4tqke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1ivqmni</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Got my nails done! Love this colour &lt;3</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivqmni</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1ivql7o</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Vacay nails</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivql7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1ivq6tw</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>🩶🩷 We have Spirit Fingers at home 😄 Night Owl Lacquer Prepared For Any &amp; All Scenarios</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivq6tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1ivq18c</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>zombie nails!!</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivq18c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1ivpyyb</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>obsessed 🩷</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1y2npjtflqke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1ivpwmo</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Polka Dots: A true test of perfectionism</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udjn821zkqke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1ivpktk</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Have been trying to recreate this Lip Smackers container for a while and I think I got pretty close!</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivpktk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1ivpnv3</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>2008 nail trends</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivpnv3/2008_nail_trends/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1ivppew</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Found a new fave magnetic!</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4i65ti1fjqke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ivpjsa</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Help with "soap nail" trend</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivpjsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ivmqab</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Hello, $40 set that I made this morning, how do you see it?🌸💘🍇</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivmqab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1ivn9rd</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Nail tech was very rough, made two of my fingers bleed, and  made the top of my nails very flat.</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivn9rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1ivo9qk</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>26 years of nail biting</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivo9qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1ivoiaj</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Pink nails with cute hearts!</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzpjdki0aqke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1ivod5m</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>I think I’m getting better.🪼🐚🐋🦈🐬🐟🌊</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivod5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1ivo9sa</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Getting my nails done makes me feel good, I should do it more often</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52w5mptd8qke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1ivo35a</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>$4 Press Ons!!</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5m4jbmd7qke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1ivo2kq</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>How to fix?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivo2kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1ivo14t</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>I’ve never shared all my recents and I always wanted to!</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivo14t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1ivnfec</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>First attempt at glass nails</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exgm0vsj2qke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1ivn89r</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Help for Kokoist order</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivn89r/help_for_kokoist_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1ivmk4y</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>does anyone know why my middle finger nail grows with a slope shape?</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivmk4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1ivl4f3</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Nail SOS.</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivl4f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1ivmiic</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Matching nail wraps for fingers and toes?</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivmiic/matching_nail_wraps_for_fingers_and_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1ivhyox</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Different effects on one hand, what do we think?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gss8lizhsoke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1ivmeuo</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Who here does their own mani and pedi at home?😅 Do you have any tips for a beginner?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivmeuo/who_here_does_their_own_mani_and_pedi_at_home_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1ivmapi</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Playing with some of my chrome powders🦄🌈</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c1c0x2j2upke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1ivlixk</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Adhering art</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ivlixk/adhering_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1iw3tgn</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Beetlejuice nails!</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw3tgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1iw3it4</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Soft pink?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tml63s3zxtke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1iw36z0</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>My tech NAILED it!</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r5mspxratke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1iw33fz</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>i just keep adding layers to this mani</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sp8084rstke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1iw1p77</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>My happy place ☺️</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ygatvg8etke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1iw1gtz</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>A Galaxy Far, Far Away</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bs89qmxbtke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1iw17ah</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Favorite polish brands that don’t chip easily?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iw17ah/favorite_polish_brands_that_dont_chip_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1ivzlw9</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Nail Polish Dupe</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivzkc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1ivz9vg</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Base coat that doesn’t peel?</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ivz9vg/base_coat_that_doesnt_peel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1ivyxmt</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>How do you all fight the FOMO? (Little Box of Horrors)</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivyxmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1ivykfe</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>fun with jelly</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivykfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1ivyixt</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Secret Society- Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt9wa1xqjske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1ivygxm</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Rainbow Nails</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivygxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1ivxn4t</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Brunhilda 💚🩷</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivxn4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1ivxjc6</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Photos Tips for Shimmer and Glitter</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ivxjc6/photos_tips_for_shimmer_and_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1ivxh1r</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>what do you call this color??</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cyjvw9s9aske1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1ivx94r</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Fresh gel manicure with tips. Kicking the nail biting habit of 30ish years. How long does it take for the nail bed to reattach and 'flatten'? It looks ridiculous now and I don't know how long I can hold out like this.</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivx94r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1ivwori</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>OPI Chopstix and Stones</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqmlznug3ske1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1ivw4bq</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Low-stakes mystery, needs solving</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivw4bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1ivw21g</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>cirque 'mood ring' velvet style live</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ogbshjgwxrke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1ivw18o</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Right as Rain 🌧️</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivw18o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1ivvwou</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Jewel of the Ball is so shifty!</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kgjdzl9owrke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1ivvt6w</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>I have been loving nail stickers lately</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivvt6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1ivuz78</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>ILNP Pine is my new favorite green</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e6e0xxworke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1ivuwed</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>From my first PPU order</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivuwed</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1ivum9j</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Game Over 🙃</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivum9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1ivukuk</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>I’ve got a Secret…</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivukuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1ivuju2</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>My boyfriend ran out of paint so he used my nail polish to paint his model plane instead</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivuju2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1ivu1yl</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Isle Be There - Kbshimmer</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivu1yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1ivtmov</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>First Mooncat order came in!</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivtmov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1ivtgiy</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>I love W7 nail polishes 🥰💅</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0vqjqnchcrke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1ivt0c3</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Gilded Gecko by Painted Polish 🦎✨</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b22virn19rke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1ivsbzm</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>root of all evil</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k9wmdbp03rke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1ivs912</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Feeling Blue 💙</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivs912</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1ivrvn7</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Idk how y'all get good photos of your nails but I finally started working on my cuticles 😄 The shade is Star destroyer by Mooncat, with their top coat and just applied their nail elixir. I love how reflective this color is!</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivrvn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1ivrc88</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Today's find</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivrc88</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1ivr3g4</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>DVN Fox Sparrow? + other assorted colors?</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ivr3g4/dvn_fox_sparrow_other_assorted_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1ivqs9z</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Can you tell what event I’m going to with this (slightly messy) mani?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hoipyj0mrqke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1ivqbtd</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>best nails for creating press-ons?</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ivqbtd/best_nails_for_creating_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1ivq5fo</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Did anyone buy Mooncat La Petite Mort?</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osdqro3umqke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1ivq4pz</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>🩶🩷 We have Spirit Fingers at home 😆 Night Owl Lacquer Prepared For Any &amp; All Scenarios</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivq4pz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1ivq1s8</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>ILNP Daydreamer 🪩💖</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/OJkdRnZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1ivpxvc</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>ILNP Pool Party is STUNNING over Essie Mint Candy Apple 😍</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivpxvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1ivpdjn</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Feeling Peachy 🍑</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0go5r50zgqke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1ivpbuy</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Does anyone know what these red spots are??</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivpbuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1ivot5r</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>The Choices We Make- EDM</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i0pqc5nocqke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1ivoizq</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>now trying What Happens Next from my first EdM haul! unreal, ethereal, talented, brilliant, amazing, etc. 🤩</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fxvg280laqke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1ivnc8q</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>I still adore Orly's 'Melting Point' collection 💙✨</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivnc8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1ivn9hz</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>ORLY Color Pass</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kb5q5hyd1qke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1ivmu2b</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Spring chaos skittle full of untrieds</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivmu2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1ivmisl</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Dollar tree finds!</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zp6t78krvpke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1ivlsgs</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>“Naiad” from Daisy Chain Polish. The swamp jelly of my dreams.</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3kzk367qpke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1ivlg53</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Emily de Molly's 4 Hours is one of the most unique polishes I've ever seen!</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivlg53</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1ivl4l8</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>What is the shelf life of nail polishes? Does brand and/or type affect shelf life?</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ivl4l8/what_is_the_shelf_life_of_nail_polishes_does/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1ivic5w</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>How did I do? Advice for better velvet effect welcome!</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/df5575x6woke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1ivi0dv</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Faded skittles &amp; doticure</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ivi0dv/faded_skittles_doticure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1iv9eam</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Gothic/Grungey/Dirty Cremes</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q1q1vc90mke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1ivgizv</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Take 2! Cosmic Polish Fantasies in Fuchsia</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/54kmccnxboke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1ive7wf</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Cosmic Polish - Fantasies in Fuchsia</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ive7wf/cosmic_polish_fantasies_in_fuchsia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1iw4nch</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>I don’t give a Dimma Damn!</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw4nch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1iw2z9u</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>I got a manicure in the color of my beloved pet's eyes</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vyhmwqurtke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1iw17ci</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>some nails i did the other day 💕✨</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2a2u5rwc9tke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1iw16xo</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Had to jump on the rose trend</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw16xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1iw0x7y</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Freestyle work! ❤️</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iw0x7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1ivxvay</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>froot 🍋🍒🍓🥝</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivxvay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1ivwlft</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>For my birthday. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u1c1xin2ske1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1ivtkjk</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Pink princess nail set by me :)</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivtkjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1ivt7o2</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>🦠 toxic ichor ☣️</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivt7o2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1ivsk0d</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Tenma Sakaki from Ultimate Exorcist Kiyoshi Manga Practice I did!</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivsk0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1ivrccc</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>my nails</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eo2e2l0svqke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1ivpunc</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Does magnetic polish count as art?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iaswwehjkqke1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1ivpui2</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>🖌️Second attempt at nail art,</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivpui2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1ivoyp8</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>New nail style I’m trying</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qv6ztftdqke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1ivogiy</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>New to press ons</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivogiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1ivn3st</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>heavenly set</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ivn3st</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1ivmsgk</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Got them done last week and I love them 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldtf6i8txpke1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1ivluld</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Sunset Ombre</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6yvaadoqpke1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1ivihab</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Do you guys like my nails. Tried chrome for the first time.</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ili23kjlxoke1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>